<commit_message>
Added 24 examples, including Toritate with floating quantifier, negation.
</commit_message>
<xml_diff>
--- a/JSeM_Toritate_20160107.xlsx
+++ b/JSeM_Toritate_20160107.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2418" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2562" uniqueCount="731">
   <si>
     <t>answer</t>
     <phoneticPr fontId="1"/>
@@ -6714,6 +6714,1000 @@
   </si>
   <si>
     <t>Toritate, -made (toritate particle), negation</t>
+  </si>
+  <si>
+    <t>《「は」とfloating quantifier》</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>学生が五人は来る。</t>
+    <rPh sb="0" eb="2">
+      <t>ガクセイ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ゴニン</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>来る学生が少なくとも五人いる。</t>
+    <rPh sb="0" eb="1">
+      <t>ク</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ガクセイ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>スク</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ゴニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「数量詞＋とりたて詞」が「〜以上」を含意する例。参考：中村ちどり (2008) 「日本の取り立て助詞と限定詞・名詞句フォーカス」、『言語と文化・文学の諸相』, pp.263-274、岩手大学人文社会科学部。</t>
+    <rPh sb="1" eb="3">
+      <t>スウリョウ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>シ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>シ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ガンイ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>レイ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>サンコウ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ナカムラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>文学部の女子学生が五人は来る。</t>
+    <rPh sb="0" eb="3">
+      <t>ブンガクブ</t>
+    </rPh>
+    <rPh sb="4" eb="8">
+      <t>ジョシガクセイ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ゴニン</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>ク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>女子学生が五人は来る。</t>
+    <rPh sb="0" eb="4">
+      <t>ジョシガクセイ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ゴニン</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>《「は」とfloating quantifier、monotonicity》</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>参考：中村ちどり (2008) 「日本の取り立て助詞と限定詞・名詞句フォーカス」、『言語と文化・文学の諸相』, pp.263-274、岩手大学人文社会科学部。</t>
+    <rPh sb="0" eb="2">
+      <t>サンコウ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ナカムラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>《「は」とfloating quantifier、否定》</t>
+    <rPh sb="25" eb="27">
+      <t>ヒテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>太郎は高級車を三台は持っている。</t>
+    <rPh sb="0" eb="2">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>コウキュウシャ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>サンダイ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>モ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>太郎が持っている高級車が少なくとも三台ある。</t>
+    <rPh sb="0" eb="2">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="8" eb="11">
+      <t>コウキュウシャ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>スク</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>サンダイ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ダイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>太郎はドイツ製の高級車を三台は持っている。</t>
+    <rPh sb="0" eb="2">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>セイ</t>
+    </rPh>
+    <rPh sb="8" eb="11">
+      <t>コウキュウシャ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>サンダイ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>モ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「否定＞数量詞＋は」の解釈。</t>
+    <rPh sb="1" eb="3">
+      <t>ヒテイ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>スウリョウ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>シ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>カイシャク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「数量詞＋は＞否定」の解釈。参考：中村ちどり (2008) 「日本の取り立て助詞と限定詞・名詞句フォーカス」、『言語と文化・文学の諸相』, pp.263-274、岩手大学人文社会科学部。</t>
+    <rPh sb="1" eb="3">
+      <t>スウリョウ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>シ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ヒテイ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>カイシャク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>《「も」とfloating quantifier》</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>《「も」とfloating quantifier、monotonicity》</t>
+  </si>
+  <si>
+    <t>《「も」とfloating quantifier、否定》</t>
+    <rPh sb="25" eb="27">
+      <t>ヒテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>学生が五人も来る。</t>
+    <rPh sb="0" eb="2">
+      <t>ガクセイ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ゴニン</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>文学部の学生が五人も来る。</t>
+    <rPh sb="0" eb="3">
+      <t>ブンガクブ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ガクセイ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ゴニン</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>太郎の結婚式には、招待客が五人は来ていなかった。</t>
+    <rPh sb="0" eb="2">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>ケッコンシキ</t>
+    </rPh>
+    <rPh sb="9" eb="12">
+      <t>ショウタイキャク</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ゴニン</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>コ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>太郎の結婚式に来ていなかった招待客が少なくとも五人いる。</t>
+    <rPh sb="0" eb="2">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>ケッコンシキ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>コ</t>
+    </rPh>
+    <rPh sb="14" eb="17">
+      <t>ショウタイキャク</t>
+    </rPh>
+    <rPh sb="18" eb="21">
+      <t>スクナクトオ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ゴニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>今日のライブには、観客が十人はいなかった。</t>
+    <rPh sb="0" eb="2">
+      <t>キョウ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>カンキャク</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ジュウニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>今日のライブにいた観客は十人未満だ。</t>
+    <rPh sb="0" eb="2">
+      <t>キョウ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>カンキャク</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ジュウニン</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ミマン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>太郎はメールを二百通は読んでいない。</t>
+    <rPh sb="0" eb="2">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="7" eb="10">
+      <t>ニヒャクツウ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>太郎が読んでいないメールが少なくとも二百通ある。</t>
+    <rPh sb="0" eb="2">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>スク</t>
+    </rPh>
+    <rPh sb="18" eb="21">
+      <t>ニヒャクツウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>学生が五人来る。</t>
+    <rPh sb="0" eb="2">
+      <t>ガクセイ</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>ゴニンク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>太郎の結婚式には、招待客が五人も来ていなかった。</t>
+    <rPh sb="0" eb="2">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>ケッコンシキ</t>
+    </rPh>
+    <rPh sb="9" eb="12">
+      <t>ショウタイキャク</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ゴニン</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>キ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>今日のライブには、観客が十人もいなかった。</t>
+    <rPh sb="0" eb="2">
+      <t>キョウ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>カンキャク</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ジュウニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「数量詞＋も＞否定」の解釈。参考：中村ちどり (2008) 「日本の取り立て助詞と限定詞・名詞句フォーカス」、『言語と文化・文学の諸相』, pp.263-274、岩手大学人文社会科学部。</t>
+    <rPh sb="1" eb="3">
+      <t>スウリョウ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>シ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ヒテイ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>カイシャク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「否定＞数量詞＋も」の解釈。</t>
+    <rPh sb="1" eb="3">
+      <t>ヒテイ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>スウリョウ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>シ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>カイシャク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>太郎の結婚式に来ていなかった招待客が五人いる。</t>
+    <rPh sb="0" eb="2">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>ケッコンシキ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="14" eb="17">
+      <t>ショウタイキャク</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ゴ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>花子は「今日のライブには、観客が百人もいた」と言った。</t>
+    <rPh sb="0" eb="2">
+      <t>ハナコ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>キョウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>カンキャク</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ヒャクニン</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>イ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「数量詞＋も」の表す、数が多いことに対する意外性。</t>
+    <rPh sb="1" eb="3">
+      <t>スウリョウ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>シ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>アラワ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>カズ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>タイ</t>
+    </rPh>
+    <rPh sb="21" eb="24">
+      <t>イガイセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>花子は、今日のライブにいた観客の数が多いと思っている。</t>
+    <rPh sb="0" eb="2">
+      <t>ハナコ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>キョウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>カンキャク</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>カズ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>オモ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>花子は「太郎の結婚式には、招待客が五人も来ていなかった」と言った。</t>
+    <rPh sb="0" eb="2">
+      <t>ハナコ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="7" eb="10">
+      <t>ケッコンシキ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ショウタイ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>キャク</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ゴニン</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>イ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>花子は、太郎の結婚式に来ていなかった招待客の数が多いと思っている。</t>
+    <rPh sb="0" eb="2">
+      <t>ハナコ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="7" eb="10">
+      <t>ケッコンシキ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="18" eb="21">
+      <t>ショウタイキャク</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>カズ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>オモ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>花子は「今日のライブには、観客が十人もいなかった」と言った。</t>
+    <rPh sb="0" eb="2">
+      <t>ハナコ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>キョウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>カンキャク</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>ジュウ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ヒャクニン</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>イ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>花子は、今日のライブにいた観客の数が少ないと思っている。</t>
+    <rPh sb="0" eb="2">
+      <t>ハナコ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>キョウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>カンキャク</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>カズ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>スク</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>オモ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「否定＞数量詞＋も」の解釈。「数量詞＋も」の表す数が少ないことに対する意外性。</t>
+    <rPh sb="15" eb="17">
+      <t>スウリョウ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>シ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>アラワ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>カズ</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>スク</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>タイ</t>
+    </rPh>
+    <rPh sb="35" eb="38">
+      <t>イガイセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「数量詞＋も＞否定」の解釈。「数量詞＋も」の表す、数が多いことに対する意外性。</t>
+    <rPh sb="1" eb="3">
+      <t>スウリョウ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>シ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ヒテイ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>カイシャク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>太郎は高級車を三台も持っている。</t>
+    <rPh sb="0" eb="2">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>コウキュウシャ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>サンダイ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>モ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>太郎は高級車を三台持っている。</t>
+    <rPh sb="0" eb="2">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>コウキュウシャ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>サンダイ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>モ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>太郎はドイツ製の高級車を三台も持っている。</t>
+    <rPh sb="0" eb="2">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>セイ</t>
+    </rPh>
+    <rPh sb="8" eb="11">
+      <t>コウキュウシャ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>サンダイ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>モ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>太郎はメールを二百通も読んでいない。</t>
+    <rPh sb="0" eb="2">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="7" eb="10">
+      <t>ニヒャクツウ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>太郎が読んでいないメールが二百通ある。</t>
+    <rPh sb="0" eb="2">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="13" eb="16">
+      <t>ニヒャクツウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>花子が「太郎は高級車を三台も持っている」と言った。</t>
+    <rPh sb="0" eb="2">
+      <t>ハナコ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="7" eb="10">
+      <t>コウキュウシャ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>サンダイ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>イ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>花子は、太郎が持っている高級車の数が多いと思っている。</t>
+    <rPh sb="0" eb="2">
+      <t>ハナコ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="12" eb="15">
+      <t>コウキュウシャ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>カズ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>オモ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>花子は「太郎はメールを二百通も読んでいない」と言った。</t>
+    <rPh sb="0" eb="2">
+      <t>ハナコ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="11" eb="14">
+      <t>ニヒャクツウ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>イ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>花子は、太郎が読んでいないメールの数が多いと思っている。</t>
+    <rPh sb="0" eb="2">
+      <t>ハナコ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>カズ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>オモ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>太郎は車を二台は持っていない。</t>
+    <rPh sb="0" eb="2">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>コウキュウシャ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ニダイ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>モ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>太郎が持っている車は二台未満である。</t>
+    <rPh sb="0" eb="2">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>コウキュウシャ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ニダイ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ミマン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>太郎は車を二台も持っていない。</t>
+    <rPh sb="0" eb="2">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>クルマ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ニダイ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>モ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>太郎が持っている車の数は二台未満だ。</t>
+    <rPh sb="0" eb="2">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>クルマ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>カズ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ニダイ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ミマン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>花子は「太郎は車を二台も持っていない」と言った。</t>
+    <rPh sb="0" eb="2">
+      <t>ハナコ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>クルマ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ニダイ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>イ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>花子は、太郎が持っている車の数が少ないと思っている。</t>
+    <rPh sb="0" eb="2">
+      <t>ハナコ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>タロウ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>クルマ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>カズ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>スク</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>オモ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Toritate, -mo (toritate particle), floating quantifier</t>
+  </si>
+  <si>
+    <t>Toritate, -mo (toritate particle), floating quantifier, negation</t>
+  </si>
+  <si>
+    <t>Toritate, -wa (toritate particle), floating quantifier</t>
+  </si>
+  <si>
+    <t>Toritate, -wa (toritate particle), floating quantifier, negation</t>
+  </si>
+  <si>
+    <t>《「までは」と否定のスコープ》</t>
+    <rPh sb="7" eb="9">
+      <t>ヒテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>unknown</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>unknown</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「ない＞までは」の解釈。参考：茂木俊伸 (1999)「とりたて詞「まで」「さえ」について―否定との関わりから―」『日本語と日本文学』28，pp.(左)27-36，筑波大学国語国文学会．</t>
+    <rPh sb="9" eb="11">
+      <t>カイシャク</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>サンコウ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>モギ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>トシノブ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>太郎は花子までは評価していない。</t>
+    <rPh sb="8" eb="10">
+      <t>ヒョウカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>花子は太郎にまではチョコレートをあげなかった。</t>
+    <rPh sb="0" eb="2">
+      <t>ハナコ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>タロウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -6806,8 +7800,66 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="783">
+  <cellStyleXfs count="841">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -7627,7 +8679,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="783">
+  <cellStyles count="841">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -8019,6 +9071,35 @@
     <cellStyle name="ハイパーリンク" xfId="777" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="779" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="781" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="783" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="785" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="787" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="789" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="791" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="793" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="795" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="797" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="799" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="801" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="803" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="805" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="807" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="809" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="811" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="813" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="815" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="817" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="819" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="821" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="823" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="825" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="827" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="829" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="831" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="833" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="835" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="837" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="839" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -8411,6 +9492,35 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="778" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="780" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="782" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="784" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="786" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="788" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="790" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="792" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="794" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="796" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="798" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="800" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="802" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="804" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="806" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="808" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="810" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="812" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="814" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="816" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="818" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="820" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="822" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="824" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="826" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="828" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="830" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="832" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="834" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="836" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="838" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="840" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -8739,11 +9849,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K356"/>
+  <dimension ref="A1:K380"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A334" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F336" sqref="F336"/>
+      <pane ySplit="1" topLeftCell="A370" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A378" sqref="A378"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -16730,6 +17840,486 @@
         <v>657</v>
       </c>
     </row>
+    <row r="357" spans="1:8" ht="65">
+      <c r="A357" s="5" t="s">
+        <v>725</v>
+      </c>
+      <c r="C357" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="D357" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="E357" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F357" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="G357" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="H357" s="2" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="358" spans="1:8" ht="65">
+      <c r="A358" s="5" t="s">
+        <v>725</v>
+      </c>
+      <c r="C358" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="D358" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="E358" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F358" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="G358" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="H358" s="2" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="359" spans="1:8" ht="65">
+      <c r="A359" s="5" t="s">
+        <v>665</v>
+      </c>
+      <c r="C359" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D359" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="F359" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="G359" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="H359" s="1" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="360" spans="1:8" ht="50">
+      <c r="A360" s="5" t="s">
+        <v>671</v>
+      </c>
+      <c r="C360" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D360" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="F360" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="G360" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="H360" s="1" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="361" spans="1:8" ht="65">
+      <c r="A361" s="5" t="s">
+        <v>673</v>
+      </c>
+      <c r="C361" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D361" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="F361" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="G361" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="H361" s="1" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="362" spans="1:8" ht="50">
+      <c r="A362" s="5" t="s">
+        <v>673</v>
+      </c>
+      <c r="C362" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D362" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="F362" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="G362" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="H362" s="1" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="363" spans="1:8" ht="65">
+      <c r="A363" s="5" t="s">
+        <v>665</v>
+      </c>
+      <c r="C363" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D363" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="F363" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="G363" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="H363" s="1" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="364" spans="1:8" ht="50">
+      <c r="A364" s="5" t="s">
+        <v>671</v>
+      </c>
+      <c r="C364" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D364" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="F364" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="G364" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="H364" s="1" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="365" spans="1:8" ht="65">
+      <c r="A365" s="5" t="s">
+        <v>673</v>
+      </c>
+      <c r="C365" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D365" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="F365" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="G365" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="H365" s="1" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="366" spans="1:8" ht="50">
+      <c r="A366" s="5" t="s">
+        <v>673</v>
+      </c>
+      <c r="C366" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D366" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="F366" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="G366" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="H366" s="1" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="367" spans="1:8" ht="50">
+      <c r="A367" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="C367" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D367" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="F367" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="G367" s="1" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="368" spans="1:8" ht="50">
+      <c r="A368" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="C368" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D368" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="F368" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="G368" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="H368" s="1" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="369" spans="1:8" ht="50">
+      <c r="A369" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="C369" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D369" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="F369" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="G369" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="H369" s="1" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="370" spans="1:8" ht="65">
+      <c r="A370" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="C370" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D370" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="F370" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="G370" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="H370" s="1" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="371" spans="1:8" ht="35">
+      <c r="A371" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="C371" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D371" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="F371" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="G371" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="H371" s="1" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="372" spans="1:8" ht="35">
+      <c r="A372" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="C372" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D372" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="F372" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="G372" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="H372" s="1" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="373" spans="1:8" ht="35">
+      <c r="A373" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="C373" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D373" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="F373" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="G373" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="H373" s="1" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="374" spans="1:8" ht="35">
+      <c r="A374" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="C374" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D374" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="F374" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="G374" s="1" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="375" spans="1:8" ht="35">
+      <c r="A375" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="C375" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D375" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="F375" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="G375" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="H375" s="1" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="376" spans="1:8" ht="50">
+      <c r="A376" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="C376" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D376" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="F376" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="G376" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="H376" s="1" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="377" spans="1:8" ht="65">
+      <c r="A377" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="C377" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D377" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="F377" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="G377" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="H377" s="1" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="378" spans="1:8" ht="35">
+      <c r="A378" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="C378" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D378" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="F378" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="G378" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="H378" s="1" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="379" spans="1:8" ht="35">
+      <c r="A379" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="C379" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D379" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="F379" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="G379" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="H379" s="1" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="380" spans="1:8" ht="35">
+      <c r="A380" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="C380" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D380" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="F380" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="G380" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="H380" s="1" t="s">
+        <v>703</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <printOptions gridLines="1"/>

</xml_diff>